<commit_message>
Excel and assambler added
</commit_message>
<xml_diff>
--- a/OPtoCUMappings.xlsx
+++ b/OPtoCUMappings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abdullah\git\303\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{607AEE57-90A0-4FE1-A2EA-44B1D923CD60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB761C06-CF6E-4482-AF21-8B1B8E15970B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{C5717BC6-AC46-40EE-BBDE-F41991607320}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C5717BC6-AC46-40EE-BBDE-F41991607320}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -156,10 +158,10 @@
     <t>Value</t>
   </si>
   <si>
-    <t>1E</t>
-  </si>
-  <si>
     <t>ADDS</t>
+  </si>
+  <si>
+    <t>Hex</t>
   </si>
 </sst>
 </file>
@@ -176,7 +178,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -186,12 +188,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -208,11 +204,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -531,7 +526,7 @@
   <dimension ref="A2:L35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="A3" sqref="A2:K18"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -574,12 +569,15 @@
       <c r="K2" s="2" t="s">
         <v>40</v>
       </c>
+      <c r="L2" s="2" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="2">
@@ -607,6 +605,11 @@
         <v>0</v>
       </c>
       <c r="K3" s="2">
+        <f>J3*128+I3*64+H3*32+G3*16+F3*8+E3*4+D3*2+C3</f>
+        <v>3</v>
+      </c>
+      <c r="L3" t="str">
+        <f>DEC2HEX(K3)</f>
         <v>3</v>
       </c>
     </row>
@@ -614,7 +617,7 @@
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="2">
@@ -642,6 +645,11 @@
         <v>0</v>
       </c>
       <c r="K4" s="2">
+        <f t="shared" ref="K4:K20" si="0">J4*128+I4*64+H4*32+G4*16+F4*8+E4*4+D4*2+C4</f>
+        <v>3</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" ref="L4:L18" si="1">DEC2HEX(K4)</f>
         <v>3</v>
       </c>
     </row>
@@ -649,14 +657,14 @@
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" s="2">
         <v>0</v>
@@ -677,14 +685,19 @@
         <v>0</v>
       </c>
       <c r="K5" s="2">
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C6" s="2">
@@ -712,6 +725,11 @@
         <v>0</v>
       </c>
       <c r="K6" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
@@ -719,7 +737,7 @@
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C7" s="2">
@@ -747,6 +765,11 @@
         <v>0</v>
       </c>
       <c r="K7" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
@@ -754,7 +777,7 @@
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C8" s="2">
@@ -782,6 +805,11 @@
         <v>0</v>
       </c>
       <c r="K8" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
     </row>
@@ -789,7 +817,7 @@
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C9" s="2">
@@ -817,6 +845,11 @@
         <v>0</v>
       </c>
       <c r="K9" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
@@ -824,7 +857,7 @@
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C10" s="2">
@@ -852,6 +885,11 @@
         <v>0</v>
       </c>
       <c r="K10" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
@@ -859,7 +897,7 @@
       <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C11" s="2">
@@ -887,6 +925,11 @@
         <v>0</v>
       </c>
       <c r="K11" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
@@ -894,7 +937,7 @@
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C12" s="2">
@@ -922,6 +965,11 @@
         <v>0</v>
       </c>
       <c r="K12" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
@@ -929,7 +977,7 @@
       <c r="A13" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>29</v>
       </c>
       <c r="C13" s="2">
@@ -956,16 +1004,20 @@
       <c r="J13" s="2">
         <v>0</v>
       </c>
-      <c r="K13" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="L13" s="3"/>
+      <c r="K13" s="2">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" si="1"/>
+        <v>1E</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C14" s="2">
@@ -993,15 +1045,19 @@
         <v>0</v>
       </c>
       <c r="K14" s="2">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="L14" t="str">
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="L14" s="3"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C15" s="2">
@@ -1029,15 +1085,19 @@
         <v>0</v>
       </c>
       <c r="K15" s="2">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="L15" t="str">
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="L15" s="3"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C16" s="2">
@@ -1065,15 +1125,19 @@
         <v>0</v>
       </c>
       <c r="K16" s="2">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="L16" t="str">
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="L16" s="3"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C17" s="2">
@@ -1101,14 +1165,19 @@
         <v>1</v>
       </c>
       <c r="K17" s="2">
+        <f t="shared" si="0"/>
+        <v>128</v>
+      </c>
+      <c r="L17" t="str">
+        <f t="shared" si="1"/>
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C18" s="2">
@@ -1136,49 +1205,56 @@
         <v>0</v>
       </c>
       <c r="K18" s="2">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="L18" t="str">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B27" s="1"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B28" s="1"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B29" s="1"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B30" s="1"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B31" s="1"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B32" s="1"/>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.3">

</xml_diff>